<commit_message>
Added dehydration validation data and new references.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/Dehydration.xlsx
+++ b/data/human/adult/validation/Scenarios/Dehydration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dehydration\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD66519-35B5-4FFF-B32B-C69B2EB9E673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA71166-A630-4D4C-B934-AB20998C8AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10095" yWindow="3405" windowWidth="33825" windowHeight="19185" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28185" yWindow="3285" windowWidth="28530" windowHeight="25860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario1" sheetId="7" r:id="rId1"/>
@@ -18,16 +18,11 @@
     <sheet name="Scenario3" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="54">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -152,6 +147,9 @@
     <t>bergeronSME</t>
   </si>
   <si>
+    <t>RespirationRate</t>
+  </si>
+  <si>
     <t>Scenario2</t>
   </si>
   <si>
@@ -159,6 +157,51 @@
   </si>
   <si>
     <t>DehydrationDataRequests</t>
+  </si>
+  <si>
+    <t>SystolicArterialPressure</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>PulsePressure</t>
+  </si>
+  <si>
+    <t>CardiacOutput</t>
+  </si>
+  <si>
+    <t>L/min</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>CentralVenousPressure</t>
+  </si>
+  <si>
+    <t>HeartStrokeVolume</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>TotalFluidVolume</t>
+  </si>
+  <si>
+    <t>BloodVolume</t>
+  </si>
+  <si>
+    <t>SweatRate</t>
+  </si>
+  <si>
+    <t>mg/min</t>
+  </si>
+  <si>
+    <t>CoreTemperature</t>
+  </si>
+  <si>
+    <t>degC</t>
   </si>
 </sst>
 </file>
@@ -254,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -325,6 +368,23 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMJ11"/>
+  <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +787,7 @@
     <col min="9" max="1024" width="11.5703125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -745,7 +805,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:8" ht="129" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" ht="129" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>28</v>
       </c>
@@ -763,7 +823,7 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -781,7 +841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>0</v>
       </c>
@@ -795,7 +855,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="17"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -815,7 +875,7 @@
       </c>
       <c r="H5" s="18"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -827,7 +887,7 @@
       </c>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -835,11 +895,11 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H7" s="19"/>
     </row>
-    <row r="8" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1024" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -857,7 +917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1024" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>1</v>
       </c>
@@ -871,7 +931,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -897,27 +957,2213 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:1024" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:1024" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:1024" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2">
-        <v>91</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:1024" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="28"/>
+      <c r="AD16" s="28"/>
+      <c r="AE16" s="28"/>
+      <c r="AF16" s="28"/>
+      <c r="AG16" s="28"/>
+      <c r="AH16" s="28"/>
+      <c r="AI16" s="28"/>
+      <c r="AJ16" s="28"/>
+      <c r="AK16" s="28"/>
+      <c r="AL16" s="28"/>
+      <c r="AM16" s="28"/>
+      <c r="AN16" s="28"/>
+      <c r="AO16" s="28"/>
+      <c r="AP16" s="28"/>
+      <c r="AQ16" s="28"/>
+      <c r="AR16" s="28"/>
+      <c r="AS16" s="28"/>
+      <c r="AT16" s="28"/>
+      <c r="AU16" s="28"/>
+      <c r="AV16" s="28"/>
+      <c r="AW16" s="28"/>
+      <c r="AX16" s="28"/>
+      <c r="AY16" s="28"/>
+      <c r="AZ16" s="28"/>
+      <c r="BA16" s="28"/>
+      <c r="BB16" s="28"/>
+      <c r="BC16" s="28"/>
+      <c r="BD16" s="28"/>
+      <c r="BE16" s="28"/>
+      <c r="BF16" s="28"/>
+      <c r="BG16" s="28"/>
+      <c r="BH16" s="28"/>
+      <c r="BI16" s="28"/>
+      <c r="BJ16" s="28"/>
+      <c r="BK16" s="28"/>
+      <c r="BL16" s="28"/>
+      <c r="BM16" s="28"/>
+      <c r="BN16" s="28"/>
+      <c r="BO16" s="28"/>
+      <c r="BP16" s="28"/>
+      <c r="BQ16" s="28"/>
+      <c r="BR16" s="28"/>
+      <c r="BS16" s="28"/>
+      <c r="BT16" s="28"/>
+      <c r="BU16" s="28"/>
+      <c r="BV16" s="28"/>
+      <c r="BW16" s="28"/>
+      <c r="BX16" s="28"/>
+      <c r="BY16" s="28"/>
+      <c r="BZ16" s="28"/>
+      <c r="CA16" s="28"/>
+      <c r="CB16" s="28"/>
+      <c r="CC16" s="28"/>
+      <c r="CD16" s="28"/>
+      <c r="CE16" s="28"/>
+      <c r="CF16" s="28"/>
+      <c r="CG16" s="28"/>
+      <c r="CH16" s="28"/>
+      <c r="CI16" s="28"/>
+      <c r="CJ16" s="28"/>
+      <c r="CK16" s="28"/>
+      <c r="CL16" s="28"/>
+      <c r="CM16" s="28"/>
+      <c r="CN16" s="28"/>
+      <c r="CO16" s="28"/>
+      <c r="CP16" s="28"/>
+      <c r="CQ16" s="28"/>
+      <c r="CR16" s="28"/>
+      <c r="CS16" s="28"/>
+      <c r="CT16" s="28"/>
+      <c r="CU16" s="28"/>
+      <c r="CV16" s="28"/>
+      <c r="CW16" s="28"/>
+      <c r="CX16" s="28"/>
+      <c r="CY16" s="28"/>
+      <c r="CZ16" s="28"/>
+      <c r="DA16" s="28"/>
+      <c r="DB16" s="28"/>
+      <c r="DC16" s="28"/>
+      <c r="DD16" s="28"/>
+      <c r="DE16" s="28"/>
+      <c r="DF16" s="28"/>
+      <c r="DG16" s="28"/>
+      <c r="DH16" s="28"/>
+      <c r="DI16" s="28"/>
+      <c r="DJ16" s="28"/>
+      <c r="DK16" s="28"/>
+      <c r="DL16" s="28"/>
+      <c r="DM16" s="28"/>
+      <c r="DN16" s="28"/>
+      <c r="DO16" s="28"/>
+      <c r="DP16" s="28"/>
+      <c r="DQ16" s="28"/>
+      <c r="DR16" s="28"/>
+      <c r="DS16" s="28"/>
+      <c r="DT16" s="28"/>
+      <c r="DU16" s="28"/>
+      <c r="DV16" s="28"/>
+      <c r="DW16" s="28"/>
+      <c r="DX16" s="28"/>
+      <c r="DY16" s="28"/>
+      <c r="DZ16" s="28"/>
+      <c r="EA16" s="28"/>
+      <c r="EB16" s="28"/>
+      <c r="EC16" s="28"/>
+      <c r="ED16" s="28"/>
+      <c r="EE16" s="28"/>
+      <c r="EF16" s="28"/>
+      <c r="EG16" s="28"/>
+      <c r="EH16" s="28"/>
+      <c r="EI16" s="28"/>
+      <c r="EJ16" s="28"/>
+      <c r="EK16" s="28"/>
+      <c r="EL16" s="28"/>
+      <c r="EM16" s="28"/>
+      <c r="EN16" s="28"/>
+      <c r="EO16" s="28"/>
+      <c r="EP16" s="28"/>
+      <c r="EQ16" s="28"/>
+      <c r="ER16" s="28"/>
+      <c r="ES16" s="28"/>
+      <c r="ET16" s="28"/>
+      <c r="EU16" s="28"/>
+      <c r="EV16" s="28"/>
+      <c r="EW16" s="28"/>
+      <c r="EX16" s="28"/>
+      <c r="EY16" s="28"/>
+      <c r="EZ16" s="28"/>
+      <c r="FA16" s="28"/>
+      <c r="FB16" s="28"/>
+      <c r="FC16" s="28"/>
+      <c r="FD16" s="28"/>
+      <c r="FE16" s="28"/>
+      <c r="FF16" s="28"/>
+      <c r="FG16" s="28"/>
+      <c r="FH16" s="28"/>
+      <c r="FI16" s="28"/>
+      <c r="FJ16" s="28"/>
+      <c r="FK16" s="28"/>
+      <c r="FL16" s="28"/>
+      <c r="FM16" s="28"/>
+      <c r="FN16" s="28"/>
+      <c r="FO16" s="28"/>
+      <c r="FP16" s="28"/>
+      <c r="FQ16" s="28"/>
+      <c r="FR16" s="28"/>
+      <c r="FS16" s="28"/>
+      <c r="FT16" s="28"/>
+      <c r="FU16" s="28"/>
+      <c r="FV16" s="28"/>
+      <c r="FW16" s="28"/>
+      <c r="FX16" s="28"/>
+      <c r="FY16" s="28"/>
+      <c r="FZ16" s="28"/>
+      <c r="GA16" s="28"/>
+      <c r="GB16" s="28"/>
+      <c r="GC16" s="28"/>
+      <c r="GD16" s="28"/>
+      <c r="GE16" s="28"/>
+      <c r="GF16" s="28"/>
+      <c r="GG16" s="28"/>
+      <c r="GH16" s="28"/>
+      <c r="GI16" s="28"/>
+      <c r="GJ16" s="28"/>
+      <c r="GK16" s="28"/>
+      <c r="GL16" s="28"/>
+      <c r="GM16" s="28"/>
+      <c r="GN16" s="28"/>
+      <c r="GO16" s="28"/>
+      <c r="GP16" s="28"/>
+      <c r="GQ16" s="28"/>
+      <c r="GR16" s="28"/>
+      <c r="GS16" s="28"/>
+      <c r="GT16" s="28"/>
+      <c r="GU16" s="28"/>
+      <c r="GV16" s="28"/>
+      <c r="GW16" s="28"/>
+      <c r="GX16" s="28"/>
+      <c r="GY16" s="28"/>
+      <c r="GZ16" s="28"/>
+      <c r="HA16" s="28"/>
+      <c r="HB16" s="28"/>
+      <c r="HC16" s="28"/>
+      <c r="HD16" s="28"/>
+      <c r="HE16" s="28"/>
+      <c r="HF16" s="28"/>
+      <c r="HG16" s="28"/>
+      <c r="HH16" s="28"/>
+      <c r="HI16" s="28"/>
+      <c r="HJ16" s="28"/>
+      <c r="HK16" s="28"/>
+      <c r="HL16" s="28"/>
+      <c r="HM16" s="28"/>
+      <c r="HN16" s="28"/>
+      <c r="HO16" s="28"/>
+      <c r="HP16" s="28"/>
+      <c r="HQ16" s="28"/>
+      <c r="HR16" s="28"/>
+      <c r="HS16" s="28"/>
+      <c r="HT16" s="28"/>
+      <c r="HU16" s="28"/>
+      <c r="HV16" s="28"/>
+      <c r="HW16" s="28"/>
+      <c r="HX16" s="28"/>
+      <c r="HY16" s="28"/>
+      <c r="HZ16" s="28"/>
+      <c r="IA16" s="28"/>
+      <c r="IB16" s="28"/>
+      <c r="IC16" s="28"/>
+      <c r="ID16" s="28"/>
+      <c r="IE16" s="28"/>
+      <c r="IF16" s="28"/>
+      <c r="IG16" s="28"/>
+      <c r="IH16" s="28"/>
+      <c r="II16" s="28"/>
+      <c r="IJ16" s="28"/>
+      <c r="IK16" s="28"/>
+      <c r="IL16" s="28"/>
+      <c r="IM16" s="28"/>
+      <c r="IN16" s="28"/>
+      <c r="IO16" s="28"/>
+      <c r="IP16" s="28"/>
+      <c r="IQ16" s="28"/>
+      <c r="IR16" s="28"/>
+      <c r="IS16" s="28"/>
+      <c r="IT16" s="28"/>
+      <c r="IU16" s="28"/>
+      <c r="IV16" s="28"/>
+      <c r="IW16" s="28"/>
+      <c r="IX16" s="28"/>
+      <c r="IY16" s="28"/>
+      <c r="IZ16" s="28"/>
+      <c r="JA16" s="28"/>
+      <c r="JB16" s="28"/>
+      <c r="JC16" s="28"/>
+      <c r="JD16" s="28"/>
+      <c r="JE16" s="28"/>
+      <c r="JF16" s="28"/>
+      <c r="JG16" s="28"/>
+      <c r="JH16" s="28"/>
+      <c r="JI16" s="28"/>
+      <c r="JJ16" s="28"/>
+      <c r="JK16" s="28"/>
+      <c r="JL16" s="28"/>
+      <c r="JM16" s="28"/>
+      <c r="JN16" s="28"/>
+      <c r="JO16" s="28"/>
+      <c r="JP16" s="28"/>
+      <c r="JQ16" s="28"/>
+      <c r="JR16" s="28"/>
+      <c r="JS16" s="28"/>
+      <c r="JT16" s="28"/>
+      <c r="JU16" s="28"/>
+      <c r="JV16" s="28"/>
+      <c r="JW16" s="28"/>
+      <c r="JX16" s="28"/>
+      <c r="JY16" s="28"/>
+      <c r="JZ16" s="28"/>
+      <c r="KA16" s="28"/>
+      <c r="KB16" s="28"/>
+      <c r="KC16" s="28"/>
+      <c r="KD16" s="28"/>
+      <c r="KE16" s="28"/>
+      <c r="KF16" s="28"/>
+      <c r="KG16" s="28"/>
+      <c r="KH16" s="28"/>
+      <c r="KI16" s="28"/>
+      <c r="KJ16" s="28"/>
+      <c r="KK16" s="28"/>
+      <c r="KL16" s="28"/>
+      <c r="KM16" s="28"/>
+      <c r="KN16" s="28"/>
+      <c r="KO16" s="28"/>
+      <c r="KP16" s="28"/>
+      <c r="KQ16" s="28"/>
+      <c r="KR16" s="28"/>
+      <c r="KS16" s="28"/>
+      <c r="KT16" s="28"/>
+      <c r="KU16" s="28"/>
+      <c r="KV16" s="28"/>
+      <c r="KW16" s="28"/>
+      <c r="KX16" s="28"/>
+      <c r="KY16" s="28"/>
+      <c r="KZ16" s="28"/>
+      <c r="LA16" s="28"/>
+      <c r="LB16" s="28"/>
+      <c r="LC16" s="28"/>
+      <c r="LD16" s="28"/>
+      <c r="LE16" s="28"/>
+      <c r="LF16" s="28"/>
+      <c r="LG16" s="28"/>
+      <c r="LH16" s="28"/>
+      <c r="LI16" s="28"/>
+      <c r="LJ16" s="28"/>
+      <c r="LK16" s="28"/>
+      <c r="LL16" s="28"/>
+      <c r="LM16" s="28"/>
+      <c r="LN16" s="28"/>
+      <c r="LO16" s="28"/>
+      <c r="LP16" s="28"/>
+      <c r="LQ16" s="28"/>
+      <c r="LR16" s="28"/>
+      <c r="LS16" s="28"/>
+      <c r="LT16" s="28"/>
+      <c r="LU16" s="28"/>
+      <c r="LV16" s="28"/>
+      <c r="LW16" s="28"/>
+      <c r="LX16" s="28"/>
+      <c r="LY16" s="28"/>
+      <c r="LZ16" s="28"/>
+      <c r="MA16" s="28"/>
+      <c r="MB16" s="28"/>
+      <c r="MC16" s="28"/>
+      <c r="MD16" s="28"/>
+      <c r="ME16" s="28"/>
+      <c r="MF16" s="28"/>
+      <c r="MG16" s="28"/>
+      <c r="MH16" s="28"/>
+      <c r="MI16" s="28"/>
+      <c r="MJ16" s="28"/>
+      <c r="MK16" s="28"/>
+      <c r="ML16" s="28"/>
+      <c r="MM16" s="28"/>
+      <c r="MN16" s="28"/>
+      <c r="MO16" s="28"/>
+      <c r="MP16" s="28"/>
+      <c r="MQ16" s="28"/>
+      <c r="MR16" s="28"/>
+      <c r="MS16" s="28"/>
+      <c r="MT16" s="28"/>
+      <c r="MU16" s="28"/>
+      <c r="MV16" s="28"/>
+      <c r="MW16" s="28"/>
+      <c r="MX16" s="28"/>
+      <c r="MY16" s="28"/>
+      <c r="MZ16" s="28"/>
+      <c r="NA16" s="28"/>
+      <c r="NB16" s="28"/>
+      <c r="NC16" s="28"/>
+      <c r="ND16" s="28"/>
+      <c r="NE16" s="28"/>
+      <c r="NF16" s="28"/>
+      <c r="NG16" s="28"/>
+      <c r="NH16" s="28"/>
+      <c r="NI16" s="28"/>
+      <c r="NJ16" s="28"/>
+      <c r="NK16" s="28"/>
+      <c r="NL16" s="28"/>
+      <c r="NM16" s="28"/>
+      <c r="NN16" s="28"/>
+      <c r="NO16" s="28"/>
+      <c r="NP16" s="28"/>
+      <c r="NQ16" s="28"/>
+      <c r="NR16" s="28"/>
+      <c r="NS16" s="28"/>
+      <c r="NT16" s="28"/>
+      <c r="NU16" s="28"/>
+      <c r="NV16" s="28"/>
+      <c r="NW16" s="28"/>
+      <c r="NX16" s="28"/>
+      <c r="NY16" s="28"/>
+      <c r="NZ16" s="28"/>
+      <c r="OA16" s="28"/>
+      <c r="OB16" s="28"/>
+      <c r="OC16" s="28"/>
+      <c r="OD16" s="28"/>
+      <c r="OE16" s="28"/>
+      <c r="OF16" s="28"/>
+      <c r="OG16" s="28"/>
+      <c r="OH16" s="28"/>
+      <c r="OI16" s="28"/>
+      <c r="OJ16" s="28"/>
+      <c r="OK16" s="28"/>
+      <c r="OL16" s="28"/>
+      <c r="OM16" s="28"/>
+      <c r="ON16" s="28"/>
+      <c r="OO16" s="28"/>
+      <c r="OP16" s="28"/>
+      <c r="OQ16" s="28"/>
+      <c r="OR16" s="28"/>
+      <c r="OS16" s="28"/>
+      <c r="OT16" s="28"/>
+      <c r="OU16" s="28"/>
+      <c r="OV16" s="28"/>
+      <c r="OW16" s="28"/>
+      <c r="OX16" s="28"/>
+      <c r="OY16" s="28"/>
+      <c r="OZ16" s="28"/>
+      <c r="PA16" s="28"/>
+      <c r="PB16" s="28"/>
+      <c r="PC16" s="28"/>
+      <c r="PD16" s="28"/>
+      <c r="PE16" s="28"/>
+      <c r="PF16" s="28"/>
+      <c r="PG16" s="28"/>
+      <c r="PH16" s="28"/>
+      <c r="PI16" s="28"/>
+      <c r="PJ16" s="28"/>
+      <c r="PK16" s="28"/>
+      <c r="PL16" s="28"/>
+      <c r="PM16" s="28"/>
+      <c r="PN16" s="28"/>
+      <c r="PO16" s="28"/>
+      <c r="PP16" s="28"/>
+      <c r="PQ16" s="28"/>
+      <c r="PR16" s="28"/>
+      <c r="PS16" s="28"/>
+      <c r="PT16" s="28"/>
+      <c r="PU16" s="28"/>
+      <c r="PV16" s="28"/>
+      <c r="PW16" s="28"/>
+      <c r="PX16" s="28"/>
+      <c r="PY16" s="28"/>
+      <c r="PZ16" s="28"/>
+      <c r="QA16" s="28"/>
+      <c r="QB16" s="28"/>
+      <c r="QC16" s="28"/>
+      <c r="QD16" s="28"/>
+      <c r="QE16" s="28"/>
+      <c r="QF16" s="28"/>
+      <c r="QG16" s="28"/>
+      <c r="QH16" s="28"/>
+      <c r="QI16" s="28"/>
+      <c r="QJ16" s="28"/>
+      <c r="QK16" s="28"/>
+      <c r="QL16" s="28"/>
+      <c r="QM16" s="28"/>
+      <c r="QN16" s="28"/>
+      <c r="QO16" s="28"/>
+      <c r="QP16" s="28"/>
+      <c r="QQ16" s="28"/>
+      <c r="QR16" s="28"/>
+      <c r="QS16" s="28"/>
+      <c r="QT16" s="28"/>
+      <c r="QU16" s="28"/>
+      <c r="QV16" s="28"/>
+      <c r="QW16" s="28"/>
+      <c r="QX16" s="28"/>
+      <c r="QY16" s="28"/>
+      <c r="QZ16" s="28"/>
+      <c r="RA16" s="28"/>
+      <c r="RB16" s="28"/>
+      <c r="RC16" s="28"/>
+      <c r="RD16" s="28"/>
+      <c r="RE16" s="28"/>
+      <c r="RF16" s="28"/>
+      <c r="RG16" s="28"/>
+      <c r="RH16" s="28"/>
+      <c r="RI16" s="28"/>
+      <c r="RJ16" s="28"/>
+      <c r="RK16" s="28"/>
+      <c r="RL16" s="28"/>
+      <c r="RM16" s="28"/>
+      <c r="RN16" s="28"/>
+      <c r="RO16" s="28"/>
+      <c r="RP16" s="28"/>
+      <c r="RQ16" s="28"/>
+      <c r="RR16" s="28"/>
+      <c r="RS16" s="28"/>
+      <c r="RT16" s="28"/>
+      <c r="RU16" s="28"/>
+      <c r="RV16" s="28"/>
+      <c r="RW16" s="28"/>
+      <c r="RX16" s="28"/>
+      <c r="RY16" s="28"/>
+      <c r="RZ16" s="28"/>
+      <c r="SA16" s="28"/>
+      <c r="SB16" s="28"/>
+      <c r="SC16" s="28"/>
+      <c r="SD16" s="28"/>
+      <c r="SE16" s="28"/>
+      <c r="SF16" s="28"/>
+      <c r="SG16" s="28"/>
+      <c r="SH16" s="28"/>
+      <c r="SI16" s="28"/>
+      <c r="SJ16" s="28"/>
+      <c r="SK16" s="28"/>
+      <c r="SL16" s="28"/>
+      <c r="SM16" s="28"/>
+      <c r="SN16" s="28"/>
+      <c r="SO16" s="28"/>
+      <c r="SP16" s="28"/>
+      <c r="SQ16" s="28"/>
+      <c r="SR16" s="28"/>
+      <c r="SS16" s="28"/>
+      <c r="ST16" s="28"/>
+      <c r="SU16" s="28"/>
+      <c r="SV16" s="28"/>
+      <c r="SW16" s="28"/>
+      <c r="SX16" s="28"/>
+      <c r="SY16" s="28"/>
+      <c r="SZ16" s="28"/>
+      <c r="TA16" s="28"/>
+      <c r="TB16" s="28"/>
+      <c r="TC16" s="28"/>
+      <c r="TD16" s="28"/>
+      <c r="TE16" s="28"/>
+      <c r="TF16" s="28"/>
+      <c r="TG16" s="28"/>
+      <c r="TH16" s="28"/>
+      <c r="TI16" s="28"/>
+      <c r="TJ16" s="28"/>
+      <c r="TK16" s="28"/>
+      <c r="TL16" s="28"/>
+      <c r="TM16" s="28"/>
+      <c r="TN16" s="28"/>
+      <c r="TO16" s="28"/>
+      <c r="TP16" s="28"/>
+      <c r="TQ16" s="28"/>
+      <c r="TR16" s="28"/>
+      <c r="TS16" s="28"/>
+      <c r="TT16" s="28"/>
+      <c r="TU16" s="28"/>
+      <c r="TV16" s="28"/>
+      <c r="TW16" s="28"/>
+      <c r="TX16" s="28"/>
+      <c r="TY16" s="28"/>
+      <c r="TZ16" s="28"/>
+      <c r="UA16" s="28"/>
+      <c r="UB16" s="28"/>
+      <c r="UC16" s="28"/>
+      <c r="UD16" s="28"/>
+      <c r="UE16" s="28"/>
+      <c r="UF16" s="28"/>
+      <c r="UG16" s="28"/>
+      <c r="UH16" s="28"/>
+      <c r="UI16" s="28"/>
+      <c r="UJ16" s="28"/>
+      <c r="UK16" s="28"/>
+      <c r="UL16" s="28"/>
+      <c r="UM16" s="28"/>
+      <c r="UN16" s="28"/>
+      <c r="UO16" s="28"/>
+      <c r="UP16" s="28"/>
+      <c r="UQ16" s="28"/>
+      <c r="UR16" s="28"/>
+      <c r="US16" s="28"/>
+      <c r="UT16" s="28"/>
+      <c r="UU16" s="28"/>
+      <c r="UV16" s="28"/>
+      <c r="UW16" s="28"/>
+      <c r="UX16" s="28"/>
+      <c r="UY16" s="28"/>
+      <c r="UZ16" s="28"/>
+      <c r="VA16" s="28"/>
+      <c r="VB16" s="28"/>
+      <c r="VC16" s="28"/>
+      <c r="VD16" s="28"/>
+      <c r="VE16" s="28"/>
+      <c r="VF16" s="28"/>
+      <c r="VG16" s="28"/>
+      <c r="VH16" s="28"/>
+      <c r="VI16" s="28"/>
+      <c r="VJ16" s="28"/>
+      <c r="VK16" s="28"/>
+      <c r="VL16" s="28"/>
+      <c r="VM16" s="28"/>
+      <c r="VN16" s="28"/>
+      <c r="VO16" s="28"/>
+      <c r="VP16" s="28"/>
+      <c r="VQ16" s="28"/>
+      <c r="VR16" s="28"/>
+      <c r="VS16" s="28"/>
+      <c r="VT16" s="28"/>
+      <c r="VU16" s="28"/>
+      <c r="VV16" s="28"/>
+      <c r="VW16" s="28"/>
+      <c r="VX16" s="28"/>
+      <c r="VY16" s="28"/>
+      <c r="VZ16" s="28"/>
+      <c r="WA16" s="28"/>
+      <c r="WB16" s="28"/>
+      <c r="WC16" s="28"/>
+      <c r="WD16" s="28"/>
+      <c r="WE16" s="28"/>
+      <c r="WF16" s="28"/>
+      <c r="WG16" s="28"/>
+      <c r="WH16" s="28"/>
+      <c r="WI16" s="28"/>
+      <c r="WJ16" s="28"/>
+      <c r="WK16" s="28"/>
+      <c r="WL16" s="28"/>
+      <c r="WM16" s="28"/>
+      <c r="WN16" s="28"/>
+      <c r="WO16" s="28"/>
+      <c r="WP16" s="28"/>
+      <c r="WQ16" s="28"/>
+      <c r="WR16" s="28"/>
+      <c r="WS16" s="28"/>
+      <c r="WT16" s="28"/>
+      <c r="WU16" s="28"/>
+      <c r="WV16" s="28"/>
+      <c r="WW16" s="28"/>
+      <c r="WX16" s="28"/>
+      <c r="WY16" s="28"/>
+      <c r="WZ16" s="28"/>
+      <c r="XA16" s="28"/>
+      <c r="XB16" s="28"/>
+      <c r="XC16" s="28"/>
+      <c r="XD16" s="28"/>
+      <c r="XE16" s="28"/>
+      <c r="XF16" s="28"/>
+      <c r="XG16" s="28"/>
+      <c r="XH16" s="28"/>
+      <c r="XI16" s="28"/>
+      <c r="XJ16" s="28"/>
+      <c r="XK16" s="28"/>
+      <c r="XL16" s="28"/>
+      <c r="XM16" s="28"/>
+      <c r="XN16" s="28"/>
+      <c r="XO16" s="28"/>
+      <c r="XP16" s="28"/>
+      <c r="XQ16" s="28"/>
+      <c r="XR16" s="28"/>
+      <c r="XS16" s="28"/>
+      <c r="XT16" s="28"/>
+      <c r="XU16" s="28"/>
+      <c r="XV16" s="28"/>
+      <c r="XW16" s="28"/>
+      <c r="XX16" s="28"/>
+      <c r="XY16" s="28"/>
+      <c r="XZ16" s="28"/>
+      <c r="YA16" s="28"/>
+      <c r="YB16" s="28"/>
+      <c r="YC16" s="28"/>
+      <c r="YD16" s="28"/>
+      <c r="YE16" s="28"/>
+      <c r="YF16" s="28"/>
+      <c r="YG16" s="28"/>
+      <c r="YH16" s="28"/>
+      <c r="YI16" s="28"/>
+      <c r="YJ16" s="28"/>
+      <c r="YK16" s="28"/>
+      <c r="YL16" s="28"/>
+      <c r="YM16" s="28"/>
+      <c r="YN16" s="28"/>
+      <c r="YO16" s="28"/>
+      <c r="YP16" s="28"/>
+      <c r="YQ16" s="28"/>
+      <c r="YR16" s="28"/>
+      <c r="YS16" s="28"/>
+      <c r="YT16" s="28"/>
+      <c r="YU16" s="28"/>
+      <c r="YV16" s="28"/>
+      <c r="YW16" s="28"/>
+      <c r="YX16" s="28"/>
+      <c r="YY16" s="28"/>
+      <c r="YZ16" s="28"/>
+      <c r="ZA16" s="28"/>
+      <c r="ZB16" s="28"/>
+      <c r="ZC16" s="28"/>
+      <c r="ZD16" s="28"/>
+      <c r="ZE16" s="28"/>
+      <c r="ZF16" s="28"/>
+      <c r="ZG16" s="28"/>
+      <c r="ZH16" s="28"/>
+      <c r="ZI16" s="28"/>
+      <c r="ZJ16" s="28"/>
+      <c r="ZK16" s="28"/>
+      <c r="ZL16" s="28"/>
+      <c r="ZM16" s="28"/>
+      <c r="ZN16" s="28"/>
+      <c r="ZO16" s="28"/>
+      <c r="ZP16" s="28"/>
+      <c r="ZQ16" s="28"/>
+      <c r="ZR16" s="28"/>
+      <c r="ZS16" s="28"/>
+      <c r="ZT16" s="28"/>
+      <c r="ZU16" s="28"/>
+      <c r="ZV16" s="28"/>
+      <c r="ZW16" s="28"/>
+      <c r="ZX16" s="28"/>
+      <c r="ZY16" s="28"/>
+      <c r="ZZ16" s="28"/>
+      <c r="AAA16" s="28"/>
+      <c r="AAB16" s="28"/>
+      <c r="AAC16" s="28"/>
+      <c r="AAD16" s="28"/>
+      <c r="AAE16" s="28"/>
+      <c r="AAF16" s="28"/>
+      <c r="AAG16" s="28"/>
+      <c r="AAH16" s="28"/>
+      <c r="AAI16" s="28"/>
+      <c r="AAJ16" s="28"/>
+      <c r="AAK16" s="28"/>
+      <c r="AAL16" s="28"/>
+      <c r="AAM16" s="28"/>
+      <c r="AAN16" s="28"/>
+      <c r="AAO16" s="28"/>
+      <c r="AAP16" s="28"/>
+      <c r="AAQ16" s="28"/>
+      <c r="AAR16" s="28"/>
+      <c r="AAS16" s="28"/>
+      <c r="AAT16" s="28"/>
+      <c r="AAU16" s="28"/>
+      <c r="AAV16" s="28"/>
+      <c r="AAW16" s="28"/>
+      <c r="AAX16" s="28"/>
+      <c r="AAY16" s="28"/>
+      <c r="AAZ16" s="28"/>
+      <c r="ABA16" s="28"/>
+      <c r="ABB16" s="28"/>
+      <c r="ABC16" s="28"/>
+      <c r="ABD16" s="28"/>
+      <c r="ABE16" s="28"/>
+      <c r="ABF16" s="28"/>
+      <c r="ABG16" s="28"/>
+      <c r="ABH16" s="28"/>
+      <c r="ABI16" s="28"/>
+      <c r="ABJ16" s="28"/>
+      <c r="ABK16" s="28"/>
+      <c r="ABL16" s="28"/>
+      <c r="ABM16" s="28"/>
+      <c r="ABN16" s="28"/>
+      <c r="ABO16" s="28"/>
+      <c r="ABP16" s="28"/>
+      <c r="ABQ16" s="28"/>
+      <c r="ABR16" s="28"/>
+      <c r="ABS16" s="28"/>
+      <c r="ABT16" s="28"/>
+      <c r="ABU16" s="28"/>
+      <c r="ABV16" s="28"/>
+      <c r="ABW16" s="28"/>
+      <c r="ABX16" s="28"/>
+      <c r="ABY16" s="28"/>
+      <c r="ABZ16" s="28"/>
+      <c r="ACA16" s="28"/>
+      <c r="ACB16" s="28"/>
+      <c r="ACC16" s="28"/>
+      <c r="ACD16" s="28"/>
+      <c r="ACE16" s="28"/>
+      <c r="ACF16" s="28"/>
+      <c r="ACG16" s="28"/>
+      <c r="ACH16" s="28"/>
+      <c r="ACI16" s="28"/>
+      <c r="ACJ16" s="28"/>
+      <c r="ACK16" s="28"/>
+      <c r="ACL16" s="28"/>
+      <c r="ACM16" s="28"/>
+      <c r="ACN16" s="28"/>
+      <c r="ACO16" s="28"/>
+      <c r="ACP16" s="28"/>
+      <c r="ACQ16" s="28"/>
+      <c r="ACR16" s="28"/>
+      <c r="ACS16" s="28"/>
+      <c r="ACT16" s="28"/>
+      <c r="ACU16" s="28"/>
+      <c r="ACV16" s="28"/>
+      <c r="ACW16" s="28"/>
+      <c r="ACX16" s="28"/>
+      <c r="ACY16" s="28"/>
+      <c r="ACZ16" s="28"/>
+      <c r="ADA16" s="28"/>
+      <c r="ADB16" s="28"/>
+      <c r="ADC16" s="28"/>
+      <c r="ADD16" s="28"/>
+      <c r="ADE16" s="28"/>
+      <c r="ADF16" s="28"/>
+      <c r="ADG16" s="28"/>
+      <c r="ADH16" s="28"/>
+      <c r="ADI16" s="28"/>
+      <c r="ADJ16" s="28"/>
+      <c r="ADK16" s="28"/>
+      <c r="ADL16" s="28"/>
+      <c r="ADM16" s="28"/>
+      <c r="ADN16" s="28"/>
+      <c r="ADO16" s="28"/>
+      <c r="ADP16" s="28"/>
+      <c r="ADQ16" s="28"/>
+      <c r="ADR16" s="28"/>
+      <c r="ADS16" s="28"/>
+      <c r="ADT16" s="28"/>
+      <c r="ADU16" s="28"/>
+      <c r="ADV16" s="28"/>
+      <c r="ADW16" s="28"/>
+      <c r="ADX16" s="28"/>
+      <c r="ADY16" s="28"/>
+      <c r="ADZ16" s="28"/>
+      <c r="AEA16" s="28"/>
+      <c r="AEB16" s="28"/>
+      <c r="AEC16" s="28"/>
+      <c r="AED16" s="28"/>
+      <c r="AEE16" s="28"/>
+      <c r="AEF16" s="28"/>
+      <c r="AEG16" s="28"/>
+      <c r="AEH16" s="28"/>
+      <c r="AEI16" s="28"/>
+      <c r="AEJ16" s="28"/>
+      <c r="AEK16" s="28"/>
+      <c r="AEL16" s="28"/>
+      <c r="AEM16" s="28"/>
+      <c r="AEN16" s="28"/>
+      <c r="AEO16" s="28"/>
+      <c r="AEP16" s="28"/>
+      <c r="AEQ16" s="28"/>
+      <c r="AER16" s="28"/>
+      <c r="AES16" s="28"/>
+      <c r="AET16" s="28"/>
+      <c r="AEU16" s="28"/>
+      <c r="AEV16" s="28"/>
+      <c r="AEW16" s="28"/>
+      <c r="AEX16" s="28"/>
+      <c r="AEY16" s="28"/>
+      <c r="AEZ16" s="28"/>
+      <c r="AFA16" s="28"/>
+      <c r="AFB16" s="28"/>
+      <c r="AFC16" s="28"/>
+      <c r="AFD16" s="28"/>
+      <c r="AFE16" s="28"/>
+      <c r="AFF16" s="28"/>
+      <c r="AFG16" s="28"/>
+      <c r="AFH16" s="28"/>
+      <c r="AFI16" s="28"/>
+      <c r="AFJ16" s="28"/>
+      <c r="AFK16" s="28"/>
+      <c r="AFL16" s="28"/>
+      <c r="AFM16" s="28"/>
+      <c r="AFN16" s="28"/>
+      <c r="AFO16" s="28"/>
+      <c r="AFP16" s="28"/>
+      <c r="AFQ16" s="28"/>
+      <c r="AFR16" s="28"/>
+      <c r="AFS16" s="28"/>
+      <c r="AFT16" s="28"/>
+      <c r="AFU16" s="28"/>
+      <c r="AFV16" s="28"/>
+      <c r="AFW16" s="28"/>
+      <c r="AFX16" s="28"/>
+      <c r="AFY16" s="28"/>
+      <c r="AFZ16" s="28"/>
+      <c r="AGA16" s="28"/>
+      <c r="AGB16" s="28"/>
+      <c r="AGC16" s="28"/>
+      <c r="AGD16" s="28"/>
+      <c r="AGE16" s="28"/>
+      <c r="AGF16" s="28"/>
+      <c r="AGG16" s="28"/>
+      <c r="AGH16" s="28"/>
+      <c r="AGI16" s="28"/>
+      <c r="AGJ16" s="28"/>
+      <c r="AGK16" s="28"/>
+      <c r="AGL16" s="28"/>
+      <c r="AGM16" s="28"/>
+      <c r="AGN16" s="28"/>
+      <c r="AGO16" s="28"/>
+      <c r="AGP16" s="28"/>
+      <c r="AGQ16" s="28"/>
+      <c r="AGR16" s="28"/>
+      <c r="AGS16" s="28"/>
+      <c r="AGT16" s="28"/>
+      <c r="AGU16" s="28"/>
+      <c r="AGV16" s="28"/>
+      <c r="AGW16" s="28"/>
+      <c r="AGX16" s="28"/>
+      <c r="AGY16" s="28"/>
+      <c r="AGZ16" s="28"/>
+      <c r="AHA16" s="28"/>
+      <c r="AHB16" s="28"/>
+      <c r="AHC16" s="28"/>
+      <c r="AHD16" s="28"/>
+      <c r="AHE16" s="28"/>
+      <c r="AHF16" s="28"/>
+      <c r="AHG16" s="28"/>
+      <c r="AHH16" s="28"/>
+      <c r="AHI16" s="28"/>
+      <c r="AHJ16" s="28"/>
+      <c r="AHK16" s="28"/>
+      <c r="AHL16" s="28"/>
+      <c r="AHM16" s="28"/>
+      <c r="AHN16" s="28"/>
+      <c r="AHO16" s="28"/>
+      <c r="AHP16" s="28"/>
+      <c r="AHQ16" s="28"/>
+      <c r="AHR16" s="28"/>
+      <c r="AHS16" s="28"/>
+      <c r="AHT16" s="28"/>
+      <c r="AHU16" s="28"/>
+      <c r="AHV16" s="28"/>
+      <c r="AHW16" s="28"/>
+      <c r="AHX16" s="28"/>
+      <c r="AHY16" s="28"/>
+      <c r="AHZ16" s="28"/>
+      <c r="AIA16" s="28"/>
+      <c r="AIB16" s="28"/>
+      <c r="AIC16" s="28"/>
+      <c r="AID16" s="28"/>
+      <c r="AIE16" s="28"/>
+      <c r="AIF16" s="28"/>
+      <c r="AIG16" s="28"/>
+      <c r="AIH16" s="28"/>
+      <c r="AII16" s="28"/>
+      <c r="AIJ16" s="28"/>
+      <c r="AIK16" s="28"/>
+      <c r="AIL16" s="28"/>
+      <c r="AIM16" s="28"/>
+      <c r="AIN16" s="28"/>
+      <c r="AIO16" s="28"/>
+      <c r="AIP16" s="28"/>
+      <c r="AIQ16" s="28"/>
+      <c r="AIR16" s="28"/>
+      <c r="AIS16" s="28"/>
+      <c r="AIT16" s="28"/>
+      <c r="AIU16" s="28"/>
+      <c r="AIV16" s="28"/>
+      <c r="AIW16" s="28"/>
+      <c r="AIX16" s="28"/>
+      <c r="AIY16" s="28"/>
+      <c r="AIZ16" s="28"/>
+      <c r="AJA16" s="28"/>
+      <c r="AJB16" s="28"/>
+      <c r="AJC16" s="28"/>
+      <c r="AJD16" s="28"/>
+      <c r="AJE16" s="28"/>
+      <c r="AJF16" s="28"/>
+      <c r="AJG16" s="28"/>
+      <c r="AJH16" s="28"/>
+      <c r="AJI16" s="28"/>
+      <c r="AJJ16" s="28"/>
+      <c r="AJK16" s="28"/>
+      <c r="AJL16" s="28"/>
+      <c r="AJM16" s="28"/>
+      <c r="AJN16" s="28"/>
+      <c r="AJO16" s="28"/>
+      <c r="AJP16" s="28"/>
+      <c r="AJQ16" s="28"/>
+      <c r="AJR16" s="28"/>
+      <c r="AJS16" s="28"/>
+      <c r="AJT16" s="28"/>
+      <c r="AJU16" s="28"/>
+      <c r="AJV16" s="28"/>
+      <c r="AJW16" s="28"/>
+      <c r="AJX16" s="28"/>
+      <c r="AJY16" s="28"/>
+      <c r="AJZ16" s="28"/>
+      <c r="AKA16" s="28"/>
+      <c r="AKB16" s="28"/>
+      <c r="AKC16" s="28"/>
+      <c r="AKD16" s="28"/>
+      <c r="AKE16" s="28"/>
+      <c r="AKF16" s="28"/>
+      <c r="AKG16" s="28"/>
+      <c r="AKH16" s="28"/>
+      <c r="AKI16" s="28"/>
+      <c r="AKJ16" s="28"/>
+      <c r="AKK16" s="28"/>
+      <c r="AKL16" s="28"/>
+      <c r="AKM16" s="28"/>
+      <c r="AKN16" s="28"/>
+      <c r="AKO16" s="28"/>
+      <c r="AKP16" s="28"/>
+      <c r="AKQ16" s="28"/>
+      <c r="AKR16" s="28"/>
+      <c r="AKS16" s="28"/>
+      <c r="AKT16" s="28"/>
+      <c r="AKU16" s="28"/>
+      <c r="AKV16" s="28"/>
+      <c r="AKW16" s="28"/>
+      <c r="AKX16" s="28"/>
+      <c r="AKY16" s="28"/>
+      <c r="AKZ16" s="28"/>
+      <c r="ALA16" s="28"/>
+      <c r="ALB16" s="28"/>
+      <c r="ALC16" s="28"/>
+      <c r="ALD16" s="28"/>
+      <c r="ALE16" s="28"/>
+      <c r="ALF16" s="28"/>
+      <c r="ALG16" s="28"/>
+      <c r="ALH16" s="28"/>
+      <c r="ALI16" s="28"/>
+      <c r="ALJ16" s="28"/>
+      <c r="ALK16" s="28"/>
+      <c r="ALL16" s="28"/>
+      <c r="ALM16" s="28"/>
+      <c r="ALN16" s="28"/>
+      <c r="ALO16" s="28"/>
+      <c r="ALP16" s="28"/>
+      <c r="ALQ16" s="28"/>
+      <c r="ALR16" s="28"/>
+      <c r="ALS16" s="28"/>
+      <c r="ALT16" s="28"/>
+      <c r="ALU16" s="28"/>
+      <c r="ALV16" s="28"/>
+      <c r="ALW16" s="28"/>
+      <c r="ALX16" s="28"/>
+      <c r="ALY16" s="28"/>
+      <c r="ALZ16" s="28"/>
+      <c r="AMA16" s="28"/>
+      <c r="AMB16" s="28"/>
+      <c r="AMC16" s="28"/>
+      <c r="AMD16" s="28"/>
+      <c r="AME16" s="28"/>
+      <c r="AMF16" s="28"/>
+      <c r="AMG16" s="28"/>
+      <c r="AMH16" s="28"/>
+      <c r="AMI16" s="28"/>
+      <c r="AMJ16" s="28"/>
+    </row>
+    <row r="17" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="17"/>
+    </row>
+    <row r="20" spans="1:1024" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="28"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="28"/>
+      <c r="AB20" s="28"/>
+      <c r="AC20" s="28"/>
+      <c r="AD20" s="28"/>
+      <c r="AE20" s="28"/>
+      <c r="AF20" s="28"/>
+      <c r="AG20" s="28"/>
+      <c r="AH20" s="28"/>
+      <c r="AI20" s="28"/>
+      <c r="AJ20" s="28"/>
+      <c r="AK20" s="28"/>
+      <c r="AL20" s="28"/>
+      <c r="AM20" s="28"/>
+      <c r="AN20" s="28"/>
+      <c r="AO20" s="28"/>
+      <c r="AP20" s="28"/>
+      <c r="AQ20" s="28"/>
+      <c r="AR20" s="28"/>
+      <c r="AS20" s="28"/>
+      <c r="AT20" s="28"/>
+      <c r="AU20" s="28"/>
+      <c r="AV20" s="28"/>
+      <c r="AW20" s="28"/>
+      <c r="AX20" s="28"/>
+      <c r="AY20" s="28"/>
+      <c r="AZ20" s="28"/>
+      <c r="BA20" s="28"/>
+      <c r="BB20" s="28"/>
+      <c r="BC20" s="28"/>
+      <c r="BD20" s="28"/>
+      <c r="BE20" s="28"/>
+      <c r="BF20" s="28"/>
+      <c r="BG20" s="28"/>
+      <c r="BH20" s="28"/>
+      <c r="BI20" s="28"/>
+      <c r="BJ20" s="28"/>
+      <c r="BK20" s="28"/>
+      <c r="BL20" s="28"/>
+      <c r="BM20" s="28"/>
+      <c r="BN20" s="28"/>
+      <c r="BO20" s="28"/>
+      <c r="BP20" s="28"/>
+      <c r="BQ20" s="28"/>
+      <c r="BR20" s="28"/>
+      <c r="BS20" s="28"/>
+      <c r="BT20" s="28"/>
+      <c r="BU20" s="28"/>
+      <c r="BV20" s="28"/>
+      <c r="BW20" s="28"/>
+      <c r="BX20" s="28"/>
+      <c r="BY20" s="28"/>
+      <c r="BZ20" s="28"/>
+      <c r="CA20" s="28"/>
+      <c r="CB20" s="28"/>
+      <c r="CC20" s="28"/>
+      <c r="CD20" s="28"/>
+      <c r="CE20" s="28"/>
+      <c r="CF20" s="28"/>
+      <c r="CG20" s="28"/>
+      <c r="CH20" s="28"/>
+      <c r="CI20" s="28"/>
+      <c r="CJ20" s="28"/>
+      <c r="CK20" s="28"/>
+      <c r="CL20" s="28"/>
+      <c r="CM20" s="28"/>
+      <c r="CN20" s="28"/>
+      <c r="CO20" s="28"/>
+      <c r="CP20" s="28"/>
+      <c r="CQ20" s="28"/>
+      <c r="CR20" s="28"/>
+      <c r="CS20" s="28"/>
+      <c r="CT20" s="28"/>
+      <c r="CU20" s="28"/>
+      <c r="CV20" s="28"/>
+      <c r="CW20" s="28"/>
+      <c r="CX20" s="28"/>
+      <c r="CY20" s="28"/>
+      <c r="CZ20" s="28"/>
+      <c r="DA20" s="28"/>
+      <c r="DB20" s="28"/>
+      <c r="DC20" s="28"/>
+      <c r="DD20" s="28"/>
+      <c r="DE20" s="28"/>
+      <c r="DF20" s="28"/>
+      <c r="DG20" s="28"/>
+      <c r="DH20" s="28"/>
+      <c r="DI20" s="28"/>
+      <c r="DJ20" s="28"/>
+      <c r="DK20" s="28"/>
+      <c r="DL20" s="28"/>
+      <c r="DM20" s="28"/>
+      <c r="DN20" s="28"/>
+      <c r="DO20" s="28"/>
+      <c r="DP20" s="28"/>
+      <c r="DQ20" s="28"/>
+      <c r="DR20" s="28"/>
+      <c r="DS20" s="28"/>
+      <c r="DT20" s="28"/>
+      <c r="DU20" s="28"/>
+      <c r="DV20" s="28"/>
+      <c r="DW20" s="28"/>
+      <c r="DX20" s="28"/>
+      <c r="DY20" s="28"/>
+      <c r="DZ20" s="28"/>
+      <c r="EA20" s="28"/>
+      <c r="EB20" s="28"/>
+      <c r="EC20" s="28"/>
+      <c r="ED20" s="28"/>
+      <c r="EE20" s="28"/>
+      <c r="EF20" s="28"/>
+      <c r="EG20" s="28"/>
+      <c r="EH20" s="28"/>
+      <c r="EI20" s="28"/>
+      <c r="EJ20" s="28"/>
+      <c r="EK20" s="28"/>
+      <c r="EL20" s="28"/>
+      <c r="EM20" s="28"/>
+      <c r="EN20" s="28"/>
+      <c r="EO20" s="28"/>
+      <c r="EP20" s="28"/>
+      <c r="EQ20" s="28"/>
+      <c r="ER20" s="28"/>
+      <c r="ES20" s="28"/>
+      <c r="ET20" s="28"/>
+      <c r="EU20" s="28"/>
+      <c r="EV20" s="28"/>
+      <c r="EW20" s="28"/>
+      <c r="EX20" s="28"/>
+      <c r="EY20" s="28"/>
+      <c r="EZ20" s="28"/>
+      <c r="FA20" s="28"/>
+      <c r="FB20" s="28"/>
+      <c r="FC20" s="28"/>
+      <c r="FD20" s="28"/>
+      <c r="FE20" s="28"/>
+      <c r="FF20" s="28"/>
+      <c r="FG20" s="28"/>
+      <c r="FH20" s="28"/>
+      <c r="FI20" s="28"/>
+      <c r="FJ20" s="28"/>
+      <c r="FK20" s="28"/>
+      <c r="FL20" s="28"/>
+      <c r="FM20" s="28"/>
+      <c r="FN20" s="28"/>
+      <c r="FO20" s="28"/>
+      <c r="FP20" s="28"/>
+      <c r="FQ20" s="28"/>
+      <c r="FR20" s="28"/>
+      <c r="FS20" s="28"/>
+      <c r="FT20" s="28"/>
+      <c r="FU20" s="28"/>
+      <c r="FV20" s="28"/>
+      <c r="FW20" s="28"/>
+      <c r="FX20" s="28"/>
+      <c r="FY20" s="28"/>
+      <c r="FZ20" s="28"/>
+      <c r="GA20" s="28"/>
+      <c r="GB20" s="28"/>
+      <c r="GC20" s="28"/>
+      <c r="GD20" s="28"/>
+      <c r="GE20" s="28"/>
+      <c r="GF20" s="28"/>
+      <c r="GG20" s="28"/>
+      <c r="GH20" s="28"/>
+      <c r="GI20" s="28"/>
+      <c r="GJ20" s="28"/>
+      <c r="GK20" s="28"/>
+      <c r="GL20" s="28"/>
+      <c r="GM20" s="28"/>
+      <c r="GN20" s="28"/>
+      <c r="GO20" s="28"/>
+      <c r="GP20" s="28"/>
+      <c r="GQ20" s="28"/>
+      <c r="GR20" s="28"/>
+      <c r="GS20" s="28"/>
+      <c r="GT20" s="28"/>
+      <c r="GU20" s="28"/>
+      <c r="GV20" s="28"/>
+      <c r="GW20" s="28"/>
+      <c r="GX20" s="28"/>
+      <c r="GY20" s="28"/>
+      <c r="GZ20" s="28"/>
+      <c r="HA20" s="28"/>
+      <c r="HB20" s="28"/>
+      <c r="HC20" s="28"/>
+      <c r="HD20" s="28"/>
+      <c r="HE20" s="28"/>
+      <c r="HF20" s="28"/>
+      <c r="HG20" s="28"/>
+      <c r="HH20" s="28"/>
+      <c r="HI20" s="28"/>
+      <c r="HJ20" s="28"/>
+      <c r="HK20" s="28"/>
+      <c r="HL20" s="28"/>
+      <c r="HM20" s="28"/>
+      <c r="HN20" s="28"/>
+      <c r="HO20" s="28"/>
+      <c r="HP20" s="28"/>
+      <c r="HQ20" s="28"/>
+      <c r="HR20" s="28"/>
+      <c r="HS20" s="28"/>
+      <c r="HT20" s="28"/>
+      <c r="HU20" s="28"/>
+      <c r="HV20" s="28"/>
+      <c r="HW20" s="28"/>
+      <c r="HX20" s="28"/>
+      <c r="HY20" s="28"/>
+      <c r="HZ20" s="28"/>
+      <c r="IA20" s="28"/>
+      <c r="IB20" s="28"/>
+      <c r="IC20" s="28"/>
+      <c r="ID20" s="28"/>
+      <c r="IE20" s="28"/>
+      <c r="IF20" s="28"/>
+      <c r="IG20" s="28"/>
+      <c r="IH20" s="28"/>
+      <c r="II20" s="28"/>
+      <c r="IJ20" s="28"/>
+      <c r="IK20" s="28"/>
+      <c r="IL20" s="28"/>
+      <c r="IM20" s="28"/>
+      <c r="IN20" s="28"/>
+      <c r="IO20" s="28"/>
+      <c r="IP20" s="28"/>
+      <c r="IQ20" s="28"/>
+      <c r="IR20" s="28"/>
+      <c r="IS20" s="28"/>
+      <c r="IT20" s="28"/>
+      <c r="IU20" s="28"/>
+      <c r="IV20" s="28"/>
+      <c r="IW20" s="28"/>
+      <c r="IX20" s="28"/>
+      <c r="IY20" s="28"/>
+      <c r="IZ20" s="28"/>
+      <c r="JA20" s="28"/>
+      <c r="JB20" s="28"/>
+      <c r="JC20" s="28"/>
+      <c r="JD20" s="28"/>
+      <c r="JE20" s="28"/>
+      <c r="JF20" s="28"/>
+      <c r="JG20" s="28"/>
+      <c r="JH20" s="28"/>
+      <c r="JI20" s="28"/>
+      <c r="JJ20" s="28"/>
+      <c r="JK20" s="28"/>
+      <c r="JL20" s="28"/>
+      <c r="JM20" s="28"/>
+      <c r="JN20" s="28"/>
+      <c r="JO20" s="28"/>
+      <c r="JP20" s="28"/>
+      <c r="JQ20" s="28"/>
+      <c r="JR20" s="28"/>
+      <c r="JS20" s="28"/>
+      <c r="JT20" s="28"/>
+      <c r="JU20" s="28"/>
+      <c r="JV20" s="28"/>
+      <c r="JW20" s="28"/>
+      <c r="JX20" s="28"/>
+      <c r="JY20" s="28"/>
+      <c r="JZ20" s="28"/>
+      <c r="KA20" s="28"/>
+      <c r="KB20" s="28"/>
+      <c r="KC20" s="28"/>
+      <c r="KD20" s="28"/>
+      <c r="KE20" s="28"/>
+      <c r="KF20" s="28"/>
+      <c r="KG20" s="28"/>
+      <c r="KH20" s="28"/>
+      <c r="KI20" s="28"/>
+      <c r="KJ20" s="28"/>
+      <c r="KK20" s="28"/>
+      <c r="KL20" s="28"/>
+      <c r="KM20" s="28"/>
+      <c r="KN20" s="28"/>
+      <c r="KO20" s="28"/>
+      <c r="KP20" s="28"/>
+      <c r="KQ20" s="28"/>
+      <c r="KR20" s="28"/>
+      <c r="KS20" s="28"/>
+      <c r="KT20" s="28"/>
+      <c r="KU20" s="28"/>
+      <c r="KV20" s="28"/>
+      <c r="KW20" s="28"/>
+      <c r="KX20" s="28"/>
+      <c r="KY20" s="28"/>
+      <c r="KZ20" s="28"/>
+      <c r="LA20" s="28"/>
+      <c r="LB20" s="28"/>
+      <c r="LC20" s="28"/>
+      <c r="LD20" s="28"/>
+      <c r="LE20" s="28"/>
+      <c r="LF20" s="28"/>
+      <c r="LG20" s="28"/>
+      <c r="LH20" s="28"/>
+      <c r="LI20" s="28"/>
+      <c r="LJ20" s="28"/>
+      <c r="LK20" s="28"/>
+      <c r="LL20" s="28"/>
+      <c r="LM20" s="28"/>
+      <c r="LN20" s="28"/>
+      <c r="LO20" s="28"/>
+      <c r="LP20" s="28"/>
+      <c r="LQ20" s="28"/>
+      <c r="LR20" s="28"/>
+      <c r="LS20" s="28"/>
+      <c r="LT20" s="28"/>
+      <c r="LU20" s="28"/>
+      <c r="LV20" s="28"/>
+      <c r="LW20" s="28"/>
+      <c r="LX20" s="28"/>
+      <c r="LY20" s="28"/>
+      <c r="LZ20" s="28"/>
+      <c r="MA20" s="28"/>
+      <c r="MB20" s="28"/>
+      <c r="MC20" s="28"/>
+      <c r="MD20" s="28"/>
+      <c r="ME20" s="28"/>
+      <c r="MF20" s="28"/>
+      <c r="MG20" s="28"/>
+      <c r="MH20" s="28"/>
+      <c r="MI20" s="28"/>
+      <c r="MJ20" s="28"/>
+      <c r="MK20" s="28"/>
+      <c r="ML20" s="28"/>
+      <c r="MM20" s="28"/>
+      <c r="MN20" s="28"/>
+      <c r="MO20" s="28"/>
+      <c r="MP20" s="28"/>
+      <c r="MQ20" s="28"/>
+      <c r="MR20" s="28"/>
+      <c r="MS20" s="28"/>
+      <c r="MT20" s="28"/>
+      <c r="MU20" s="28"/>
+      <c r="MV20" s="28"/>
+      <c r="MW20" s="28"/>
+      <c r="MX20" s="28"/>
+      <c r="MY20" s="28"/>
+      <c r="MZ20" s="28"/>
+      <c r="NA20" s="28"/>
+      <c r="NB20" s="28"/>
+      <c r="NC20" s="28"/>
+      <c r="ND20" s="28"/>
+      <c r="NE20" s="28"/>
+      <c r="NF20" s="28"/>
+      <c r="NG20" s="28"/>
+      <c r="NH20" s="28"/>
+      <c r="NI20" s="28"/>
+      <c r="NJ20" s="28"/>
+      <c r="NK20" s="28"/>
+      <c r="NL20" s="28"/>
+      <c r="NM20" s="28"/>
+      <c r="NN20" s="28"/>
+      <c r="NO20" s="28"/>
+      <c r="NP20" s="28"/>
+      <c r="NQ20" s="28"/>
+      <c r="NR20" s="28"/>
+      <c r="NS20" s="28"/>
+      <c r="NT20" s="28"/>
+      <c r="NU20" s="28"/>
+      <c r="NV20" s="28"/>
+      <c r="NW20" s="28"/>
+      <c r="NX20" s="28"/>
+      <c r="NY20" s="28"/>
+      <c r="NZ20" s="28"/>
+      <c r="OA20" s="28"/>
+      <c r="OB20" s="28"/>
+      <c r="OC20" s="28"/>
+      <c r="OD20" s="28"/>
+      <c r="OE20" s="28"/>
+      <c r="OF20" s="28"/>
+      <c r="OG20" s="28"/>
+      <c r="OH20" s="28"/>
+      <c r="OI20" s="28"/>
+      <c r="OJ20" s="28"/>
+      <c r="OK20" s="28"/>
+      <c r="OL20" s="28"/>
+      <c r="OM20" s="28"/>
+      <c r="ON20" s="28"/>
+      <c r="OO20" s="28"/>
+      <c r="OP20" s="28"/>
+      <c r="OQ20" s="28"/>
+      <c r="OR20" s="28"/>
+      <c r="OS20" s="28"/>
+      <c r="OT20" s="28"/>
+      <c r="OU20" s="28"/>
+      <c r="OV20" s="28"/>
+      <c r="OW20" s="28"/>
+      <c r="OX20" s="28"/>
+      <c r="OY20" s="28"/>
+      <c r="OZ20" s="28"/>
+      <c r="PA20" s="28"/>
+      <c r="PB20" s="28"/>
+      <c r="PC20" s="28"/>
+      <c r="PD20" s="28"/>
+      <c r="PE20" s="28"/>
+      <c r="PF20" s="28"/>
+      <c r="PG20" s="28"/>
+      <c r="PH20" s="28"/>
+      <c r="PI20" s="28"/>
+      <c r="PJ20" s="28"/>
+      <c r="PK20" s="28"/>
+      <c r="PL20" s="28"/>
+      <c r="PM20" s="28"/>
+      <c r="PN20" s="28"/>
+      <c r="PO20" s="28"/>
+      <c r="PP20" s="28"/>
+      <c r="PQ20" s="28"/>
+      <c r="PR20" s="28"/>
+      <c r="PS20" s="28"/>
+      <c r="PT20" s="28"/>
+      <c r="PU20" s="28"/>
+      <c r="PV20" s="28"/>
+      <c r="PW20" s="28"/>
+      <c r="PX20" s="28"/>
+      <c r="PY20" s="28"/>
+      <c r="PZ20" s="28"/>
+      <c r="QA20" s="28"/>
+      <c r="QB20" s="28"/>
+      <c r="QC20" s="28"/>
+      <c r="QD20" s="28"/>
+      <c r="QE20" s="28"/>
+      <c r="QF20" s="28"/>
+      <c r="QG20" s="28"/>
+      <c r="QH20" s="28"/>
+      <c r="QI20" s="28"/>
+      <c r="QJ20" s="28"/>
+      <c r="QK20" s="28"/>
+      <c r="QL20" s="28"/>
+      <c r="QM20" s="28"/>
+      <c r="QN20" s="28"/>
+      <c r="QO20" s="28"/>
+      <c r="QP20" s="28"/>
+      <c r="QQ20" s="28"/>
+      <c r="QR20" s="28"/>
+      <c r="QS20" s="28"/>
+      <c r="QT20" s="28"/>
+      <c r="QU20" s="28"/>
+      <c r="QV20" s="28"/>
+      <c r="QW20" s="28"/>
+      <c r="QX20" s="28"/>
+      <c r="QY20" s="28"/>
+      <c r="QZ20" s="28"/>
+      <c r="RA20" s="28"/>
+      <c r="RB20" s="28"/>
+      <c r="RC20" s="28"/>
+      <c r="RD20" s="28"/>
+      <c r="RE20" s="28"/>
+      <c r="RF20" s="28"/>
+      <c r="RG20" s="28"/>
+      <c r="RH20" s="28"/>
+      <c r="RI20" s="28"/>
+      <c r="RJ20" s="28"/>
+      <c r="RK20" s="28"/>
+      <c r="RL20" s="28"/>
+      <c r="RM20" s="28"/>
+      <c r="RN20" s="28"/>
+      <c r="RO20" s="28"/>
+      <c r="RP20" s="28"/>
+      <c r="RQ20" s="28"/>
+      <c r="RR20" s="28"/>
+      <c r="RS20" s="28"/>
+      <c r="RT20" s="28"/>
+      <c r="RU20" s="28"/>
+      <c r="RV20" s="28"/>
+      <c r="RW20" s="28"/>
+      <c r="RX20" s="28"/>
+      <c r="RY20" s="28"/>
+      <c r="RZ20" s="28"/>
+      <c r="SA20" s="28"/>
+      <c r="SB20" s="28"/>
+      <c r="SC20" s="28"/>
+      <c r="SD20" s="28"/>
+      <c r="SE20" s="28"/>
+      <c r="SF20" s="28"/>
+      <c r="SG20" s="28"/>
+      <c r="SH20" s="28"/>
+      <c r="SI20" s="28"/>
+      <c r="SJ20" s="28"/>
+      <c r="SK20" s="28"/>
+      <c r="SL20" s="28"/>
+      <c r="SM20" s="28"/>
+      <c r="SN20" s="28"/>
+      <c r="SO20" s="28"/>
+      <c r="SP20" s="28"/>
+      <c r="SQ20" s="28"/>
+      <c r="SR20" s="28"/>
+      <c r="SS20" s="28"/>
+      <c r="ST20" s="28"/>
+      <c r="SU20" s="28"/>
+      <c r="SV20" s="28"/>
+      <c r="SW20" s="28"/>
+      <c r="SX20" s="28"/>
+      <c r="SY20" s="28"/>
+      <c r="SZ20" s="28"/>
+      <c r="TA20" s="28"/>
+      <c r="TB20" s="28"/>
+      <c r="TC20" s="28"/>
+      <c r="TD20" s="28"/>
+      <c r="TE20" s="28"/>
+      <c r="TF20" s="28"/>
+      <c r="TG20" s="28"/>
+      <c r="TH20" s="28"/>
+      <c r="TI20" s="28"/>
+      <c r="TJ20" s="28"/>
+      <c r="TK20" s="28"/>
+      <c r="TL20" s="28"/>
+      <c r="TM20" s="28"/>
+      <c r="TN20" s="28"/>
+      <c r="TO20" s="28"/>
+      <c r="TP20" s="28"/>
+      <c r="TQ20" s="28"/>
+      <c r="TR20" s="28"/>
+      <c r="TS20" s="28"/>
+      <c r="TT20" s="28"/>
+      <c r="TU20" s="28"/>
+      <c r="TV20" s="28"/>
+      <c r="TW20" s="28"/>
+      <c r="TX20" s="28"/>
+      <c r="TY20" s="28"/>
+      <c r="TZ20" s="28"/>
+      <c r="UA20" s="28"/>
+      <c r="UB20" s="28"/>
+      <c r="UC20" s="28"/>
+      <c r="UD20" s="28"/>
+      <c r="UE20" s="28"/>
+      <c r="UF20" s="28"/>
+      <c r="UG20" s="28"/>
+      <c r="UH20" s="28"/>
+      <c r="UI20" s="28"/>
+      <c r="UJ20" s="28"/>
+      <c r="UK20" s="28"/>
+      <c r="UL20" s="28"/>
+      <c r="UM20" s="28"/>
+      <c r="UN20" s="28"/>
+      <c r="UO20" s="28"/>
+      <c r="UP20" s="28"/>
+      <c r="UQ20" s="28"/>
+      <c r="UR20" s="28"/>
+      <c r="US20" s="28"/>
+      <c r="UT20" s="28"/>
+      <c r="UU20" s="28"/>
+      <c r="UV20" s="28"/>
+      <c r="UW20" s="28"/>
+      <c r="UX20" s="28"/>
+      <c r="UY20" s="28"/>
+      <c r="UZ20" s="28"/>
+      <c r="VA20" s="28"/>
+      <c r="VB20" s="28"/>
+      <c r="VC20" s="28"/>
+      <c r="VD20" s="28"/>
+      <c r="VE20" s="28"/>
+      <c r="VF20" s="28"/>
+      <c r="VG20" s="28"/>
+      <c r="VH20" s="28"/>
+      <c r="VI20" s="28"/>
+      <c r="VJ20" s="28"/>
+      <c r="VK20" s="28"/>
+      <c r="VL20" s="28"/>
+      <c r="VM20" s="28"/>
+      <c r="VN20" s="28"/>
+      <c r="VO20" s="28"/>
+      <c r="VP20" s="28"/>
+      <c r="VQ20" s="28"/>
+      <c r="VR20" s="28"/>
+      <c r="VS20" s="28"/>
+      <c r="VT20" s="28"/>
+      <c r="VU20" s="28"/>
+      <c r="VV20" s="28"/>
+      <c r="VW20" s="28"/>
+      <c r="VX20" s="28"/>
+      <c r="VY20" s="28"/>
+      <c r="VZ20" s="28"/>
+      <c r="WA20" s="28"/>
+      <c r="WB20" s="28"/>
+      <c r="WC20" s="28"/>
+      <c r="WD20" s="28"/>
+      <c r="WE20" s="28"/>
+      <c r="WF20" s="28"/>
+      <c r="WG20" s="28"/>
+      <c r="WH20" s="28"/>
+      <c r="WI20" s="28"/>
+      <c r="WJ20" s="28"/>
+      <c r="WK20" s="28"/>
+      <c r="WL20" s="28"/>
+      <c r="WM20" s="28"/>
+      <c r="WN20" s="28"/>
+      <c r="WO20" s="28"/>
+      <c r="WP20" s="28"/>
+      <c r="WQ20" s="28"/>
+      <c r="WR20" s="28"/>
+      <c r="WS20" s="28"/>
+      <c r="WT20" s="28"/>
+      <c r="WU20" s="28"/>
+      <c r="WV20" s="28"/>
+      <c r="WW20" s="28"/>
+      <c r="WX20" s="28"/>
+      <c r="WY20" s="28"/>
+      <c r="WZ20" s="28"/>
+      <c r="XA20" s="28"/>
+      <c r="XB20" s="28"/>
+      <c r="XC20" s="28"/>
+      <c r="XD20" s="28"/>
+      <c r="XE20" s="28"/>
+      <c r="XF20" s="28"/>
+      <c r="XG20" s="28"/>
+      <c r="XH20" s="28"/>
+      <c r="XI20" s="28"/>
+      <c r="XJ20" s="28"/>
+      <c r="XK20" s="28"/>
+      <c r="XL20" s="28"/>
+      <c r="XM20" s="28"/>
+      <c r="XN20" s="28"/>
+      <c r="XO20" s="28"/>
+      <c r="XP20" s="28"/>
+      <c r="XQ20" s="28"/>
+      <c r="XR20" s="28"/>
+      <c r="XS20" s="28"/>
+      <c r="XT20" s="28"/>
+      <c r="XU20" s="28"/>
+      <c r="XV20" s="28"/>
+      <c r="XW20" s="28"/>
+      <c r="XX20" s="28"/>
+      <c r="XY20" s="28"/>
+      <c r="XZ20" s="28"/>
+      <c r="YA20" s="28"/>
+      <c r="YB20" s="28"/>
+      <c r="YC20" s="28"/>
+      <c r="YD20" s="28"/>
+      <c r="YE20" s="28"/>
+      <c r="YF20" s="28"/>
+      <c r="YG20" s="28"/>
+      <c r="YH20" s="28"/>
+      <c r="YI20" s="28"/>
+      <c r="YJ20" s="28"/>
+      <c r="YK20" s="28"/>
+      <c r="YL20" s="28"/>
+      <c r="YM20" s="28"/>
+      <c r="YN20" s="28"/>
+      <c r="YO20" s="28"/>
+      <c r="YP20" s="28"/>
+      <c r="YQ20" s="28"/>
+      <c r="YR20" s="28"/>
+      <c r="YS20" s="28"/>
+      <c r="YT20" s="28"/>
+      <c r="YU20" s="28"/>
+      <c r="YV20" s="28"/>
+      <c r="YW20" s="28"/>
+      <c r="YX20" s="28"/>
+      <c r="YY20" s="28"/>
+      <c r="YZ20" s="28"/>
+      <c r="ZA20" s="28"/>
+      <c r="ZB20" s="28"/>
+      <c r="ZC20" s="28"/>
+      <c r="ZD20" s="28"/>
+      <c r="ZE20" s="28"/>
+      <c r="ZF20" s="28"/>
+      <c r="ZG20" s="28"/>
+      <c r="ZH20" s="28"/>
+      <c r="ZI20" s="28"/>
+      <c r="ZJ20" s="28"/>
+      <c r="ZK20" s="28"/>
+      <c r="ZL20" s="28"/>
+      <c r="ZM20" s="28"/>
+      <c r="ZN20" s="28"/>
+      <c r="ZO20" s="28"/>
+      <c r="ZP20" s="28"/>
+      <c r="ZQ20" s="28"/>
+      <c r="ZR20" s="28"/>
+      <c r="ZS20" s="28"/>
+      <c r="ZT20" s="28"/>
+      <c r="ZU20" s="28"/>
+      <c r="ZV20" s="28"/>
+      <c r="ZW20" s="28"/>
+      <c r="ZX20" s="28"/>
+      <c r="ZY20" s="28"/>
+      <c r="ZZ20" s="28"/>
+      <c r="AAA20" s="28"/>
+      <c r="AAB20" s="28"/>
+      <c r="AAC20" s="28"/>
+      <c r="AAD20" s="28"/>
+      <c r="AAE20" s="28"/>
+      <c r="AAF20" s="28"/>
+      <c r="AAG20" s="28"/>
+      <c r="AAH20" s="28"/>
+      <c r="AAI20" s="28"/>
+      <c r="AAJ20" s="28"/>
+      <c r="AAK20" s="28"/>
+      <c r="AAL20" s="28"/>
+      <c r="AAM20" s="28"/>
+      <c r="AAN20" s="28"/>
+      <c r="AAO20" s="28"/>
+      <c r="AAP20" s="28"/>
+      <c r="AAQ20" s="28"/>
+      <c r="AAR20" s="28"/>
+      <c r="AAS20" s="28"/>
+      <c r="AAT20" s="28"/>
+      <c r="AAU20" s="28"/>
+      <c r="AAV20" s="28"/>
+      <c r="AAW20" s="28"/>
+      <c r="AAX20" s="28"/>
+      <c r="AAY20" s="28"/>
+      <c r="AAZ20" s="28"/>
+      <c r="ABA20" s="28"/>
+      <c r="ABB20" s="28"/>
+      <c r="ABC20" s="28"/>
+      <c r="ABD20" s="28"/>
+      <c r="ABE20" s="28"/>
+      <c r="ABF20" s="28"/>
+      <c r="ABG20" s="28"/>
+      <c r="ABH20" s="28"/>
+      <c r="ABI20" s="28"/>
+      <c r="ABJ20" s="28"/>
+      <c r="ABK20" s="28"/>
+      <c r="ABL20" s="28"/>
+      <c r="ABM20" s="28"/>
+      <c r="ABN20" s="28"/>
+      <c r="ABO20" s="28"/>
+      <c r="ABP20" s="28"/>
+      <c r="ABQ20" s="28"/>
+      <c r="ABR20" s="28"/>
+      <c r="ABS20" s="28"/>
+      <c r="ABT20" s="28"/>
+      <c r="ABU20" s="28"/>
+      <c r="ABV20" s="28"/>
+      <c r="ABW20" s="28"/>
+      <c r="ABX20" s="28"/>
+      <c r="ABY20" s="28"/>
+      <c r="ABZ20" s="28"/>
+      <c r="ACA20" s="28"/>
+      <c r="ACB20" s="28"/>
+      <c r="ACC20" s="28"/>
+      <c r="ACD20" s="28"/>
+      <c r="ACE20" s="28"/>
+      <c r="ACF20" s="28"/>
+      <c r="ACG20" s="28"/>
+      <c r="ACH20" s="28"/>
+      <c r="ACI20" s="28"/>
+      <c r="ACJ20" s="28"/>
+      <c r="ACK20" s="28"/>
+      <c r="ACL20" s="28"/>
+      <c r="ACM20" s="28"/>
+      <c r="ACN20" s="28"/>
+      <c r="ACO20" s="28"/>
+      <c r="ACP20" s="28"/>
+      <c r="ACQ20" s="28"/>
+      <c r="ACR20" s="28"/>
+      <c r="ACS20" s="28"/>
+      <c r="ACT20" s="28"/>
+      <c r="ACU20" s="28"/>
+      <c r="ACV20" s="28"/>
+      <c r="ACW20" s="28"/>
+      <c r="ACX20" s="28"/>
+      <c r="ACY20" s="28"/>
+      <c r="ACZ20" s="28"/>
+      <c r="ADA20" s="28"/>
+      <c r="ADB20" s="28"/>
+      <c r="ADC20" s="28"/>
+      <c r="ADD20" s="28"/>
+      <c r="ADE20" s="28"/>
+      <c r="ADF20" s="28"/>
+      <c r="ADG20" s="28"/>
+      <c r="ADH20" s="28"/>
+      <c r="ADI20" s="28"/>
+      <c r="ADJ20" s="28"/>
+      <c r="ADK20" s="28"/>
+      <c r="ADL20" s="28"/>
+      <c r="ADM20" s="28"/>
+      <c r="ADN20" s="28"/>
+      <c r="ADO20" s="28"/>
+      <c r="ADP20" s="28"/>
+      <c r="ADQ20" s="28"/>
+      <c r="ADR20" s="28"/>
+      <c r="ADS20" s="28"/>
+      <c r="ADT20" s="28"/>
+      <c r="ADU20" s="28"/>
+      <c r="ADV20" s="28"/>
+      <c r="ADW20" s="28"/>
+      <c r="ADX20" s="28"/>
+      <c r="ADY20" s="28"/>
+      <c r="ADZ20" s="28"/>
+      <c r="AEA20" s="28"/>
+      <c r="AEB20" s="28"/>
+      <c r="AEC20" s="28"/>
+      <c r="AED20" s="28"/>
+      <c r="AEE20" s="28"/>
+      <c r="AEF20" s="28"/>
+      <c r="AEG20" s="28"/>
+      <c r="AEH20" s="28"/>
+      <c r="AEI20" s="28"/>
+      <c r="AEJ20" s="28"/>
+      <c r="AEK20" s="28"/>
+      <c r="AEL20" s="28"/>
+      <c r="AEM20" s="28"/>
+      <c r="AEN20" s="28"/>
+      <c r="AEO20" s="28"/>
+      <c r="AEP20" s="28"/>
+      <c r="AEQ20" s="28"/>
+      <c r="AER20" s="28"/>
+      <c r="AES20" s="28"/>
+      <c r="AET20" s="28"/>
+      <c r="AEU20" s="28"/>
+      <c r="AEV20" s="28"/>
+      <c r="AEW20" s="28"/>
+      <c r="AEX20" s="28"/>
+      <c r="AEY20" s="28"/>
+      <c r="AEZ20" s="28"/>
+      <c r="AFA20" s="28"/>
+      <c r="AFB20" s="28"/>
+      <c r="AFC20" s="28"/>
+      <c r="AFD20" s="28"/>
+      <c r="AFE20" s="28"/>
+      <c r="AFF20" s="28"/>
+      <c r="AFG20" s="28"/>
+      <c r="AFH20" s="28"/>
+      <c r="AFI20" s="28"/>
+      <c r="AFJ20" s="28"/>
+      <c r="AFK20" s="28"/>
+      <c r="AFL20" s="28"/>
+      <c r="AFM20" s="28"/>
+      <c r="AFN20" s="28"/>
+      <c r="AFO20" s="28"/>
+      <c r="AFP20" s="28"/>
+      <c r="AFQ20" s="28"/>
+      <c r="AFR20" s="28"/>
+      <c r="AFS20" s="28"/>
+      <c r="AFT20" s="28"/>
+      <c r="AFU20" s="28"/>
+      <c r="AFV20" s="28"/>
+      <c r="AFW20" s="28"/>
+      <c r="AFX20" s="28"/>
+      <c r="AFY20" s="28"/>
+      <c r="AFZ20" s="28"/>
+      <c r="AGA20" s="28"/>
+      <c r="AGB20" s="28"/>
+      <c r="AGC20" s="28"/>
+      <c r="AGD20" s="28"/>
+      <c r="AGE20" s="28"/>
+      <c r="AGF20" s="28"/>
+      <c r="AGG20" s="28"/>
+      <c r="AGH20" s="28"/>
+      <c r="AGI20" s="28"/>
+      <c r="AGJ20" s="28"/>
+      <c r="AGK20" s="28"/>
+      <c r="AGL20" s="28"/>
+      <c r="AGM20" s="28"/>
+      <c r="AGN20" s="28"/>
+      <c r="AGO20" s="28"/>
+      <c r="AGP20" s="28"/>
+      <c r="AGQ20" s="28"/>
+      <c r="AGR20" s="28"/>
+      <c r="AGS20" s="28"/>
+      <c r="AGT20" s="28"/>
+      <c r="AGU20" s="28"/>
+      <c r="AGV20" s="28"/>
+      <c r="AGW20" s="28"/>
+      <c r="AGX20" s="28"/>
+      <c r="AGY20" s="28"/>
+      <c r="AGZ20" s="28"/>
+      <c r="AHA20" s="28"/>
+      <c r="AHB20" s="28"/>
+      <c r="AHC20" s="28"/>
+      <c r="AHD20" s="28"/>
+      <c r="AHE20" s="28"/>
+      <c r="AHF20" s="28"/>
+      <c r="AHG20" s="28"/>
+      <c r="AHH20" s="28"/>
+      <c r="AHI20" s="28"/>
+      <c r="AHJ20" s="28"/>
+      <c r="AHK20" s="28"/>
+      <c r="AHL20" s="28"/>
+      <c r="AHM20" s="28"/>
+      <c r="AHN20" s="28"/>
+      <c r="AHO20" s="28"/>
+      <c r="AHP20" s="28"/>
+      <c r="AHQ20" s="28"/>
+      <c r="AHR20" s="28"/>
+      <c r="AHS20" s="28"/>
+      <c r="AHT20" s="28"/>
+      <c r="AHU20" s="28"/>
+      <c r="AHV20" s="28"/>
+      <c r="AHW20" s="28"/>
+      <c r="AHX20" s="28"/>
+      <c r="AHY20" s="28"/>
+      <c r="AHZ20" s="28"/>
+      <c r="AIA20" s="28"/>
+      <c r="AIB20" s="28"/>
+      <c r="AIC20" s="28"/>
+      <c r="AID20" s="28"/>
+      <c r="AIE20" s="28"/>
+      <c r="AIF20" s="28"/>
+      <c r="AIG20" s="28"/>
+      <c r="AIH20" s="28"/>
+      <c r="AII20" s="28"/>
+      <c r="AIJ20" s="28"/>
+      <c r="AIK20" s="28"/>
+      <c r="AIL20" s="28"/>
+      <c r="AIM20" s="28"/>
+      <c r="AIN20" s="28"/>
+      <c r="AIO20" s="28"/>
+      <c r="AIP20" s="28"/>
+      <c r="AIQ20" s="28"/>
+      <c r="AIR20" s="28"/>
+      <c r="AIS20" s="28"/>
+      <c r="AIT20" s="28"/>
+      <c r="AIU20" s="28"/>
+      <c r="AIV20" s="28"/>
+      <c r="AIW20" s="28"/>
+      <c r="AIX20" s="28"/>
+      <c r="AIY20" s="28"/>
+      <c r="AIZ20" s="28"/>
+      <c r="AJA20" s="28"/>
+      <c r="AJB20" s="28"/>
+      <c r="AJC20" s="28"/>
+      <c r="AJD20" s="28"/>
+      <c r="AJE20" s="28"/>
+      <c r="AJF20" s="28"/>
+      <c r="AJG20" s="28"/>
+      <c r="AJH20" s="28"/>
+      <c r="AJI20" s="28"/>
+      <c r="AJJ20" s="28"/>
+      <c r="AJK20" s="28"/>
+      <c r="AJL20" s="28"/>
+      <c r="AJM20" s="28"/>
+      <c r="AJN20" s="28"/>
+      <c r="AJO20" s="28"/>
+      <c r="AJP20" s="28"/>
+      <c r="AJQ20" s="28"/>
+      <c r="AJR20" s="28"/>
+      <c r="AJS20" s="28"/>
+      <c r="AJT20" s="28"/>
+      <c r="AJU20" s="28"/>
+      <c r="AJV20" s="28"/>
+      <c r="AJW20" s="28"/>
+      <c r="AJX20" s="28"/>
+      <c r="AJY20" s="28"/>
+      <c r="AJZ20" s="28"/>
+      <c r="AKA20" s="28"/>
+      <c r="AKB20" s="28"/>
+      <c r="AKC20" s="28"/>
+      <c r="AKD20" s="28"/>
+      <c r="AKE20" s="28"/>
+      <c r="AKF20" s="28"/>
+      <c r="AKG20" s="28"/>
+      <c r="AKH20" s="28"/>
+      <c r="AKI20" s="28"/>
+      <c r="AKJ20" s="28"/>
+      <c r="AKK20" s="28"/>
+      <c r="AKL20" s="28"/>
+      <c r="AKM20" s="28"/>
+      <c r="AKN20" s="28"/>
+      <c r="AKO20" s="28"/>
+      <c r="AKP20" s="28"/>
+      <c r="AKQ20" s="28"/>
+      <c r="AKR20" s="28"/>
+      <c r="AKS20" s="28"/>
+      <c r="AKT20" s="28"/>
+      <c r="AKU20" s="28"/>
+      <c r="AKV20" s="28"/>
+      <c r="AKW20" s="28"/>
+      <c r="AKX20" s="28"/>
+      <c r="AKY20" s="28"/>
+      <c r="AKZ20" s="28"/>
+      <c r="ALA20" s="28"/>
+      <c r="ALB20" s="28"/>
+      <c r="ALC20" s="28"/>
+      <c r="ALD20" s="28"/>
+      <c r="ALE20" s="28"/>
+      <c r="ALF20" s="28"/>
+      <c r="ALG20" s="28"/>
+      <c r="ALH20" s="28"/>
+      <c r="ALI20" s="28"/>
+      <c r="ALJ20" s="28"/>
+      <c r="ALK20" s="28"/>
+      <c r="ALL20" s="28"/>
+      <c r="ALM20" s="28"/>
+      <c r="ALN20" s="28"/>
+      <c r="ALO20" s="28"/>
+      <c r="ALP20" s="28"/>
+      <c r="ALQ20" s="28"/>
+      <c r="ALR20" s="28"/>
+      <c r="ALS20" s="28"/>
+      <c r="ALT20" s="28"/>
+      <c r="ALU20" s="28"/>
+      <c r="ALV20" s="28"/>
+      <c r="ALW20" s="28"/>
+      <c r="ALX20" s="28"/>
+      <c r="ALY20" s="28"/>
+      <c r="ALZ20" s="28"/>
+      <c r="AMA20" s="28"/>
+      <c r="AMB20" s="28"/>
+      <c r="AMC20" s="28"/>
+      <c r="AMD20" s="28"/>
+      <c r="AME20" s="28"/>
+      <c r="AMF20" s="28"/>
+      <c r="AMG20" s="28"/>
+      <c r="AMH20" s="28"/>
+      <c r="AMI20" s="28"/>
+      <c r="AMJ20" s="28"/>
+    </row>
+    <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -949,7 +3195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C22A4B-7DC3-4468-B3AD-DF3C2884C93E}">
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -990,7 +3236,7 @@
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="5" t="s">
@@ -1074,7 +3320,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H7" s="19"/>
     </row>
@@ -1189,7 +3435,7 @@
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +3475,7 @@
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="5" t="s">
@@ -1313,7 +3559,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H7" s="19"/>
     </row>

</xml_diff>

<commit_message>
Add dehydration documentation.  Add new scenario for drinking salt water after dehydration. Updates to dehydration validation.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/Dehydration.xlsx
+++ b/data/human/adult/validation/Scenarios/Dehydration.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\ec_engine\data\human\adult\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dehydration\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC4C3DB-47A4-4869-8B6A-EB1E94F5C867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58F755B-B5BF-42AD-9A6A-9A0874446E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28770" windowHeight="17250" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15045" yWindow="7350" windowWidth="23130" windowHeight="19155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mild" sheetId="7" r:id="rId1"/>
-    <sheet name="Moderate" sheetId="8" r:id="rId2"/>
-    <sheet name="Severe" sheetId="9" r:id="rId3"/>
+    <sheet name="Scenario0" sheetId="11" r:id="rId1"/>
+    <sheet name="Scenario1" sheetId="7" r:id="rId2"/>
+    <sheet name="Sceanrio2" sheetId="8" r:id="rId3"/>
+    <sheet name="Scenario3" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="43">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -114,46 +115,61 @@
     <t>Mild Dehydration</t>
   </si>
   <si>
+    <t>mild dehydration</t>
+  </si>
+  <si>
+    <t>Moderate Dehydration</t>
+  </si>
+  <si>
+    <t>moderate dehydration</t>
+  </si>
+  <si>
+    <t>bergeronSME</t>
+  </si>
+  <si>
+    <t>DehydrationDataRequests</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>{ "PatientAction": { "Assessment": { "Type": "Urinalysis" }}}</t>
+  </si>
+  <si>
+    <t>For urine color validation</t>
+  </si>
+  <si>
+    <t>Scenario0</t>
+  </si>
+  <si>
+    <t>Scenario1</t>
+  </si>
+  <si>
+    <t>Scenario2</t>
+  </si>
+  <si>
+    <t>Scenario3</t>
+  </si>
+  <si>
     <t>{ "PatientCondition": {
         "Dehydration": {
           "Severity": {
             "Scalar0To1": {
-              "Value": 0.3
+              "Value": 0.7
             } } } }
 }</t>
-  </si>
-  <si>
-    <t>mild dehydration</t>
-  </si>
-  <si>
-    <t>Moderate Dehydration</t>
-  </si>
-  <si>
-    <t>moderate dehydration</t>
   </si>
   <si>
     <t>{ "PatientCondition": {
         "Dehydration": {
           "Severity": {
             "Scalar0To1": {
-              "Value": 0.6
+              "Value": 0.5
             } } } }
 }</t>
   </si>
   <si>
-    <t>bergeronSME</t>
-  </si>
-  <si>
-    <t>DehydrationDataRequests</t>
-  </si>
-  <si>
-    <t>Mild</t>
-  </si>
-  <si>
-    <t>Moderate</t>
-  </si>
-  <si>
-    <t>Severe</t>
+    <t>healthy</t>
   </si>
 </sst>
 </file>
@@ -300,6 +316,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -310,16 +335,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,11 +718,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMJ11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61A7EA3-2DB4-4952-AEFD-37C48922A5ED}">
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,52 +739,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="129" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="24"/>
+      <c r="A2" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="20"/>
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="F2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
@@ -776,17 +792,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>0</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="4"/>
       <c r="H4" s="17"/>
     </row>
@@ -803,24 +817,24 @@
       <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="21" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="18" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="18"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -829,22 +843,22 @@
       <c r="D7" s="10"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="18"/>
+      <c r="G7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
@@ -856,80 +870,97 @@
       <c r="A9" s="12">
         <v>1</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13"/>
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2">
         <v>91</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
+      <c r="F12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -941,11 +972,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C22A4B-7DC3-4468-B3AD-DF3C2884C93E}">
-  <dimension ref="A1:AMJ11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,52 +993,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="129" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="24"/>
+      <c r="A2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="20"/>
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="F2" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1019,13 +1050,13 @@
       <c r="A4" s="10">
         <v>0</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="B4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="4"/>
       <c r="H4" s="17"/>
     </row>
@@ -1042,24 +1073,24 @@
       <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="21" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="18" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="18"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -1068,22 +1099,22 @@
       <c r="D7" s="10"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="18"/>
+      <c r="G7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1095,80 +1126,97 @@
       <c r="A9" s="12">
         <v>1</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13"/>
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2">
         <v>91</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
+      <c r="F12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B10:F10"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1180,11 +1228,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B282E4DC-0B8D-487E-A497-DD64F028D134}">
-  <dimension ref="A1:AMJ11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C22A4B-7DC3-4468-B3AD-DF3C2884C93E}">
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B4" sqref="B4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,52 +1249,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="129" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="24"/>
+      <c r="A2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="20"/>
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="F2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1258,13 +1306,13 @@
       <c r="A4" s="10">
         <v>0</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="B4" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="4"/>
       <c r="H4" s="17"/>
     </row>
@@ -1281,24 +1329,24 @@
       <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="21" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="18" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="18"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -1307,22 +1355,22 @@
       <c r="D7" s="10"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="18"/>
+      <c r="G7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1334,72 +1382,83 @@
       <c r="A9" s="12">
         <v>1</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13"/>
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2">
         <v>91</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
+      <c r="F12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:H2"/>
+  <mergeCells count="15">
+    <mergeCell ref="B10:F10"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
@@ -1408,6 +1467,268 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B282E4DC-0B8D-487E-A497-DD64F028D134}">
+  <dimension ref="A1:AMJ12"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15" style="8" customWidth="1"/>
+    <col min="4" max="4" width="25" style="8" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" style="9" customWidth="1"/>
+    <col min="9" max="1024" width="11.5703125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" ht="129" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>0</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>1</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2">
+        <v>91</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>